<commit_message>
brand filter added category
</commit_message>
<xml_diff>
--- a/public/export/sample_categories.xlsx
+++ b/public/export/sample_categories.xlsx
@@ -275,10 +275,10 @@
     <t>Product</t>
   </si>
   <si>
-    <t>**** Sparetime Hobby ****</t>
-  </si>
-  <si>
-    <t>Sparetime Hobby</t>
+    <t>**** Sparetime Hobby111 ****</t>
+  </si>
+  <si>
+    <t>Sparetime Hobby111</t>
   </si>
   <si>
     <t>Fritidshobby</t>
@@ -4964,6 +4964,9 @@
       <c r="D37" t="s">
         <v>86</v>
       </c>
+      <c r="E37">
+        <v>25.0</v>
+      </c>
       <c r="F37" t="s">
         <v>87</v>
       </c>
@@ -11862,10 +11865,10 @@
         <v>993</v>
       </c>
       <c r="C412" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="D412" t="s">
-        <v>668</v>
+        <v>988</v>
       </c>
       <c r="F412" t="s">
         <v>994</v>
@@ -11882,10 +11885,10 @@
         <v>993</v>
       </c>
       <c r="C413" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="D413" t="s">
-        <v>988</v>
+        <v>668</v>
       </c>
       <c r="F413" t="s">
         <v>994</v>

</xml_diff>